<commit_message>
working parsers for rmc and gga
</commit_message>
<xml_diff>
--- a/Protocol/src/ApplicationLayer/AppComponents/ExcelToAppComponent/Eolian_auriga/components.xlsx
+++ b/Protocol/src/ApplicationLayer/AppComponents/ExcelToAppComponent/Eolian_auriga/components.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Github\Eolian-Telemetria-Auriga\Protocol\src\ExcelToAppComponent\Eolian_auriga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dante\Desktop\Eolian\Eolian-Auriga-backend\Protocol\src\ApplicationLayer\AppComponents\ExcelToAppComponent\Eolian_auriga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02D1117-43D3-4C4C-A836-455D004E9B93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8291B9BC-67BB-4779-892A-F1241BE13F16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="1464" windowWidth="18360" windowHeight="10536" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inversor_der" sheetId="2" r:id="rId1"/>
     <sheet name="inversor_izq" sheetId="3" r:id="rId2"/>
     <sheet name="bms" sheetId="4" r:id="rId3"/>
-    <sheet name="bms_temp" sheetId="5" r:id="rId4"/>
-    <sheet name="bms_volt" sheetId="6" r:id="rId5"/>
-    <sheet name="luces" sheetId="11" r:id="rId6"/>
-    <sheet name="marchas" sheetId="12" r:id="rId7"/>
-    <sheet name="mppt1" sheetId="7" r:id="rId8"/>
-    <sheet name="mppt2" sheetId="8" r:id="rId9"/>
-    <sheet name="mppt3" sheetId="9" r:id="rId10"/>
-    <sheet name="mppt4" sheetId="10" r:id="rId11"/>
-    <sheet name="acelerometro" sheetId="14" r:id="rId12"/>
+    <sheet name="gps" sheetId="15" r:id="rId4"/>
+    <sheet name="bms_temp" sheetId="5" r:id="rId5"/>
+    <sheet name="bms_volt" sheetId="6" r:id="rId6"/>
+    <sheet name="luces" sheetId="11" r:id="rId7"/>
+    <sheet name="marchas" sheetId="12" r:id="rId8"/>
+    <sheet name="mppt1" sheetId="7" r:id="rId9"/>
+    <sheet name="mppt2" sheetId="8" r:id="rId10"/>
+    <sheet name="mppt3" sheetId="9" r:id="rId11"/>
+    <sheet name="mppt4" sheetId="10" r:id="rId12"/>
+    <sheet name="acelerometro" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="127">
   <si>
     <t>SOC</t>
   </si>
@@ -396,6 +397,27 @@
   </si>
   <si>
     <t>marcha</t>
+  </si>
+  <si>
+    <t>LATITUD</t>
+  </si>
+  <si>
+    <t>ANGULO_LATITUD</t>
+  </si>
+  <si>
+    <t>ORIENTACION_LATITUD</t>
+  </si>
+  <si>
+    <t>LONGITUD</t>
+  </si>
+  <si>
+    <t>ANGULO_LONGITUD</t>
+  </si>
+  <si>
+    <t>ORIENTACION_LONGITUD</t>
+  </si>
+  <si>
+    <t>00.0000</t>
   </si>
 </sst>
 </file>
@@ -445,10 +467,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,9 +758,9 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -753,7 +776,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -769,7 +792,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -785,7 +808,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
     </row>
   </sheetData>
@@ -795,6 +818,99 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FA06F7-36F4-4A7C-BFEF-6657330EB921}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="B2">
+        <v>-0.1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>129.9</v>
+      </c>
+      <c r="B3">
+        <v>49.9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>129.9</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B05DA13-A9BE-4CFA-8886-CBABF9CA7C76}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -802,9 +918,9 @@
       <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -830,7 +946,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>-0.1</v>
       </c>
@@ -856,7 +972,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>129.9</v>
       </c>
@@ -887,7 +1003,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C67BBD65-0C1C-49CF-A495-01A07240720A}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -895,9 +1011,9 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -923,7 +1039,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>-0.1</v>
       </c>
@@ -949,7 +1065,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>129.9</v>
       </c>
@@ -980,7 +1096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B6D6F58-ED9D-4990-A7A0-D169D3D50964}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -988,7 +1104,7 @@
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1002,9 +1118,9 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1020,7 +1136,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1036,7 +1152,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1061,13 +1177,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B547D1-632A-4F3B-9A3A-887796921B5F}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1230,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1161,7 +1277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>100</v>
       </c>
@@ -1214,6 +1330,84 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1E0C48-4D9D-42FB-AD62-5ACFC1B922CE}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>99.999899999999997</v>
+      </c>
+      <c r="B3">
+        <v>90</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>99.999899999999997</v>
+      </c>
+      <c r="E3">
+        <v>180</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A2 D2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39D22A6-69A3-4C78-81BF-9DE38D1DB719}">
   <dimension ref="A1:BH3"/>
   <sheetViews>
@@ -1221,9 +1415,9 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1405,7 +1599,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>-9.9</v>
       </c>
@@ -1587,7 +1781,7 @@
         <v>-9.9</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>89.9</v>
       </c>
@@ -1775,7 +1969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF960A0-F629-434E-B8CE-7DE56A6AF799}">
   <dimension ref="A1:AD3"/>
   <sheetViews>
@@ -1783,9 +1977,9 @@
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -1877,7 +2071,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2.4990000000000001</v>
       </c>
@@ -1969,7 +2163,7 @@
         <v>2.4990000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4.2990000000000004</v>
       </c>
@@ -2067,7 +2261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E95E6DB-D9D5-48CC-A526-6D3DD8646156}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2075,9 +2269,9 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -2097,7 +2291,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2117,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2142,7 +2336,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD999E06-E2C4-46D8-ABB0-7BAF398617DF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2150,14 +2344,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2167,7 +2361,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60ED005C-EE4F-4655-A412-314A8EE2E525}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -2175,9 +2369,9 @@
       <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -2203,7 +2397,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>-0.1</v>
       </c>
@@ -2229,100 +2423,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>129.9</v>
-      </c>
-      <c r="B3">
-        <v>49.9</v>
-      </c>
-      <c r="C3" s="2">
-        <v>129.9</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FA06F7-36F4-4A7C-BFEF-6657330EB921}">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>-0.1</v>
-      </c>
-      <c r="B2">
-        <v>-0.1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>-0.1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>129.9</v>
       </c>

</xml_diff>